<commit_message>
Issue no. 66 @1411156163
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>id</t>
   </si>
@@ -148,12 +148,6 @@
   </si>
   <si>
     <t>03.08.2014: Nord-/ Südhimmel prüfen.</t>
-  </si>
-  <si>
-    <t>outline-Attribut für BodyAreal</t>
-  </si>
-  <si>
-    <t>outline-Attribut für CatalogDS9</t>
   </si>
   <si>
     <t>Optional, Default-Wert true.</t>
@@ -211,10 +205,37 @@
     <t>fov-Attribut für Circle-Elemente prüfen/ einführen.</t>
   </si>
   <si>
-    <t>Verwendung von JTS anstell von ListCutter prüfen/ einführen.</t>
-  </si>
-  <si>
     <t>Skalenstriche vor DialDay nicht orthogonal zur Tangente</t>
+  </si>
+  <si>
+    <t>09.09.2014: Für Catalog*Record umgesetzt.</t>
+  </si>
+  <si>
+    <t>contour-Attribut für CatalogDS9</t>
+  </si>
+  <si>
+    <t>contour-Attribut für BodyAreal</t>
+  </si>
+  <si>
+    <t>Methode directionOfScaleMarkValue in BodySun implementiert.</t>
+  </si>
+  <si>
+    <t>09.09.2014: Reproduzierbar mit plantdials.xml.</t>
+  </si>
+  <si>
+    <t>peer-Parameter für Konstruktor Body* prüfen/ entfernen</t>
+  </si>
+  <si>
+    <t>Graduation* auf ein Element reduzieren</t>
+  </si>
+  <si>
+    <t>Differenzierung von Parametern für GraduationSpan, -Half, -Full über name-Attribut.</t>
+  </si>
+  <si>
+    <t>13.09.2014: division-Attribut von GraduationSpan nach DialDegree ändern.</t>
+  </si>
+  <si>
+    <t>Verwendung von JTS anstelle von ListCutter prüfen/ einführen.</t>
   </si>
 </sst>
 </file>
@@ -591,7 +612,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,457 +645,493 @@
     </row>
     <row r="5" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D5" s="6">
+        <v>1030</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="3">
+        <v>41893</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="6">
         <v>1028</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="E6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="3">
         <v>41891</v>
       </c>
-    </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="6">
-        <v>1025</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="3">
-        <v>41869</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>41895</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D7" s="6">
-        <v>1022</v>
+        <v>1029</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="H7" s="3">
-        <v>41854</v>
+        <v>41891</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" s="6">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="H8" s="3">
-        <v>41854</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+        <v>41869</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9" s="6">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H9" s="3">
         <v>41854</v>
       </c>
     </row>
-    <row r="10" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" s="6">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="H10" s="3">
-        <v>41841</v>
+        <v>41854</v>
+      </c>
+      <c r="I10" s="2">
+        <v>41891</v>
       </c>
     </row>
     <row r="11" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D11" s="6">
+        <v>1024</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="3">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" s="6">
+        <v>1026</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="3">
+        <v>41841</v>
+      </c>
+      <c r="I12" s="2">
+        <v>41901</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="6">
         <v>1027</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="3">
         <v>41841</v>
-      </c>
-    </row>
-    <row r="12" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D12" s="6">
-        <v>1019</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="3">
-        <v>41724</v>
-      </c>
-    </row>
-    <row r="13" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D13" s="6">
-        <v>1020</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="3">
-        <v>41724</v>
       </c>
     </row>
     <row r="14" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D14" s="6">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H14" s="3">
         <v>41724</v>
       </c>
     </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D15" s="6">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="H15" s="3">
-        <v>41576</v>
-      </c>
-    </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+        <v>41724</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D16" s="6">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="H16" s="3">
-        <v>41484</v>
+        <v>41724</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="6">
+        <v>1018</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3">
+        <v>41576</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="6">
+        <v>1017</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="3">
+        <v>41484</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="6">
         <v>1016</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H19" s="3">
         <v>41363</v>
       </c>
     </row>
-    <row r="18" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D18" s="6">
+    <row r="20" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D20" s="6">
         <v>1015</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H20" s="3">
         <v>41362</v>
       </c>
     </row>
-    <row r="19" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D19" s="6">
+    <row r="21" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="6">
         <v>1014</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H21" s="3">
         <v>41229</v>
       </c>
     </row>
-    <row r="20" spans="4:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D20" s="6">
+    <row r="22" spans="4:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="D22" s="6">
         <v>1013</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H22" s="3">
         <v>41092</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="6">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="6">
         <v>1012</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H23" s="3">
         <v>41028</v>
       </c>
     </row>
-    <row r="22" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D22" s="6">
+    <row r="24" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D24" s="6">
         <v>1010</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H24" s="3">
         <v>40959</v>
       </c>
     </row>
-    <row r="23" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D23" s="6">
+    <row r="25" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D25" s="6">
         <v>1011</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="F25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="3">
         <v>40959</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="6">
-        <v>1008</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="3">
-        <v>40956</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D25" s="6">
-        <v>1009</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="3">
-        <v>40956</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="6">
+        <v>1008</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="3">
+        <v>40956</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="D27" s="6">
+        <v>1009</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="3">
+        <v>40956</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="6">
         <v>1007</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H28" s="3">
         <v>40947</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D27" s="6">
-        <v>1006</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="3">
-        <v>40869</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="D28" s="6">
-        <v>1005</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="3">
-        <v>40866</v>
       </c>
     </row>
     <row r="29" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D29" s="6">
+        <v>1006</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="3">
+        <v>40869</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="D30" s="6">
+        <v>1005</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="3">
+        <v>40866</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D31" s="6">
         <v>1004</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H31" s="3">
         <v>40794</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="6">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="6">
         <v>1003</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H32" s="3">
         <v>40763</v>
       </c>
     </row>
-    <row r="31" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D31" s="6">
+    <row r="33" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D33" s="6">
         <v>1002</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H33" s="3">
         <v>40506</v>
       </c>
     </row>
-    <row r="32" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D32" s="6">
+    <row r="34" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D34" s="6">
         <v>1001</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H34" s="3">
         <v>39122</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="6">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="6">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" s="6">
         <v>1031</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36" s="6">
         <v>1032</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" s="6">
         <v>1033</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" s="6">
         <v>1034</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D39" s="6">
         <v>1035</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D40" s="6">
         <v>1036</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41" s="6">
         <v>1037</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D42" s="6">
         <v>1038</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D43" s="6">
         <v>1039</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44" s="6">
         <v>1040</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D45" s="6">
         <v>1041</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D46" s="6">
         <v>1042</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D47" s="6">
         <v>1043</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D48" s="6">
         <v>1044</v>
       </c>
@@ -1102,18 +1159,18 @@
   <sheetData>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>0.72</v>
@@ -1125,7 +1182,7 @@
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>0.96</v>
@@ -1136,7 +1193,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <f>(E7-E6)/(D10-1)</f>
@@ -1145,7 +1202,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>12</v>
@@ -1153,13 +1210,13 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Issue no. 67 @1413490269
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -229,13 +229,51 @@
     <t>Graduation* auf ein Element reduzieren</t>
   </si>
   <si>
-    <t>Differenzierung von Parametern für GraduationSpan, -Half, -Full über name-Attribut.</t>
-  </si>
-  <si>
-    <t>13.09.2014: division-Attribut von GraduationSpan nach DialDegree ändern.</t>
-  </si>
-  <si>
     <t>Verwendung von JTS anstelle von ListCutter prüfen/ einführen.</t>
+  </si>
+  <si>
+    <t>Circle* auf JTS umstellen</t>
+  </si>
+  <si>
+    <t>Klasse ist Alpha, Omega optional, Mapping wegen Namenskonflikt mit Circle* einführen.</t>
+  </si>
+  <si>
+    <t>Alpha/ Omega optional, default 0/ 359 bzw. -90/ 90 (prefs), mapping wegen Namenskonflikt mit Epoch einführen</t>
+  </si>
+  <si>
+    <t>Klasse Epoch optimieren</t>
+  </si>
+  <si>
+    <t>Wertebereiche für A/ O in Circle* einführen</t>
+  </si>
+  <si>
+    <t>CircleType Begin/ End nach Alpha/ Omega ändern</t>
+  </si>
+  <si>
+    <t>Element-Class-mapping, beide optional, default aus preferences.</t>
+  </si>
+  <si>
+    <t>Differenzierung von preferences für GraduationSpan, -Half, -Full über name-Attribut, division-Attribut von GraduationSpan nach DialDegree ändern.</t>
+  </si>
+  <si>
+    <t>19.09.2014: fieldofview-Attribut für CircleType eingeführt.</t>
+  </si>
+  <si>
+    <t>Graduation posistion/ direction optimieren</t>
+  </si>
+  <si>
+    <t>12.10.2014: Verschiedene Optimierungen (Namen, rotate, apply() in Graduation, for-Schleife in DialDeg). Graduation umbenannt in Scaleline.</t>
+  </si>
+  <si>
+    <t>Bezeichnungen prüfen, rotate in Graduation und directionOfScaleMarkN prüfen, Aufruf von direction Of* in postionOf* prüfen. Graduation umbenennen in Scaleline.
+Startpunkt für Skalenstrich vor Aufruf von Scaleline einstellen, Koordinatensystem mit x-Achse parallel zum Skalenstrich ausrichten.</t>
+  </si>
+  <si>
+    <t>-180 bis 360 excl. Im Modell, ! 360&gt;O-A in Applikation.
+Verwendung von MapTo0To360Range in bspw, CircleParallel.list() prüfen; sind u.U. bsolet.</t>
+  </si>
+  <si>
+    <t>16.09.2014: Notwendig für klassenspezifische Attribute, bspw. type, die nicht im Scope der Parent-Klasse BodyOrbitalType liegen.</t>
   </si>
 </sst>
 </file>
@@ -287,7 +325,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -302,6 +339,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,530 +649,595 @@
   <dimension ref="D4:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="7"/>
+    <col min="4" max="4" width="9.140625" style="6"/>
     <col min="5" max="7" width="45.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="11.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="4" t="s">
+    <row r="4" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D5" s="6">
+    <row r="5" spans="4:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="D5" s="5">
+        <v>1035</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="2">
+        <v>41924</v>
+      </c>
+      <c r="I5" s="2">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="D6" s="5">
+        <v>1033</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="2">
+        <v>41918</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
+        <v>1034</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="2">
+        <v>41918</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" s="5">
+        <v>1031</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="2">
+        <v>41917</v>
+      </c>
+      <c r="I8" s="2">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D9" s="5">
+        <v>1032</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="2">
+        <v>41917</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="D10" s="5">
         <v>1030</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="2">
+        <v>41893</v>
+      </c>
+      <c r="I10" s="2">
+        <v>41924</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="5">
+        <v>1028</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="2">
+        <v>41891</v>
+      </c>
+      <c r="I11" s="2">
+        <v>41895</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D12" s="5">
+        <v>1029</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="2">
+        <v>41891</v>
+      </c>
+      <c r="I12" s="2">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="5">
+        <v>1025</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="2">
+        <v>41869</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="5">
+        <v>1022</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="2">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="5">
+        <v>1023</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="2">
+        <v>41854</v>
+      </c>
+      <c r="I15" s="2">
+        <v>41891</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D16" s="5">
+        <v>1024</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="2">
+        <v>41854</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="5">
+        <v>1026</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="3">
-        <v>41893</v>
-      </c>
-    </row>
-    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D6" s="6">
-        <v>1028</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="3">
-        <v>41891</v>
-      </c>
-      <c r="I6" s="2">
-        <v>41895</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D7" s="6">
-        <v>1029</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="3">
-        <v>41891</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="6">
-        <v>1025</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="3">
-        <v>41869</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="6">
-        <v>1022</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="3">
-        <v>41854</v>
-      </c>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="6">
-        <v>1023</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="3">
-        <v>41854</v>
-      </c>
-      <c r="I10" s="2">
-        <v>41891</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D11" s="6">
-        <v>1024</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="3">
-        <v>41854</v>
-      </c>
-    </row>
-    <row r="12" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D12" s="6">
-        <v>1026</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="H17" s="2">
         <v>41841</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I17" s="2">
         <v>41901</v>
       </c>
     </row>
-    <row r="13" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D13" s="6">
+    <row r="18" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="5">
         <v>1027</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="3">
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="2">
         <v>41841</v>
       </c>
-    </row>
-    <row r="14" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D14" s="6">
+      <c r="I18" s="2">
+        <v>41901</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D19" s="5">
         <v>1019</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H19" s="2">
         <v>41724</v>
       </c>
     </row>
-    <row r="15" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D15" s="6">
+    <row r="20" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D20" s="5">
         <v>1020</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H20" s="2">
         <v>41724</v>
       </c>
     </row>
-    <row r="16" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D16" s="6">
+    <row r="21" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D21" s="5">
         <v>1021</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H21" s="2">
         <v>41724</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="6">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="5">
         <v>1018</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H22" s="2">
         <v>41576</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="6">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="5">
         <v>1017</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H23" s="2">
         <v>41484</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="6">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="5">
         <v>1016</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H24" s="2">
         <v>41363</v>
       </c>
     </row>
-    <row r="20" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D20" s="6">
+    <row r="25" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D25" s="5">
         <v>1015</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H25" s="2">
         <v>41362</v>
       </c>
     </row>
-    <row r="21" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D21" s="6">
+    <row r="26" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D26" s="5">
         <v>1014</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H26" s="2">
         <v>41229</v>
       </c>
     </row>
-    <row r="22" spans="4:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D22" s="6">
+    <row r="27" spans="4:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="D27" s="5">
         <v>1013</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H27" s="2">
         <v>41092</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="6">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="5">
         <v>1012</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H28" s="2">
         <v>41028</v>
       </c>
     </row>
-    <row r="24" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D24" s="6">
+    <row r="29" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" s="5">
         <v>1010</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H29" s="2">
         <v>40959</v>
       </c>
     </row>
-    <row r="25" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D25" s="6">
+    <row r="30" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D30" s="5">
         <v>1011</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H30" s="2">
         <v>40959</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="6">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="5">
         <v>1008</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H31" s="2">
         <v>40956</v>
       </c>
     </row>
-    <row r="27" spans="4:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D27" s="6">
+    <row r="32" spans="4:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="D32" s="5">
         <v>1009</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H32" s="2">
         <v>40956</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="6">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="5">
         <v>1007</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H33" s="2">
         <v>40947</v>
       </c>
     </row>
-    <row r="29" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D29" s="6">
+    <row r="34" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D34" s="5">
         <v>1006</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H34" s="2">
         <v>40869</v>
       </c>
     </row>
-    <row r="30" spans="4:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="D30" s="6">
+    <row r="35" spans="4:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="D35" s="5">
         <v>1005</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H35" s="2">
         <v>40866</v>
       </c>
     </row>
-    <row r="31" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D31" s="6">
+    <row r="36" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36" s="5">
         <v>1004</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H36" s="2">
         <v>40794</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="6">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D37" s="5">
         <v>1003</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H37" s="2">
         <v>40763</v>
       </c>
     </row>
-    <row r="33" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D33" s="6">
+    <row r="38" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D38" s="5">
         <v>1002</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H38" s="2">
         <v>40506</v>
       </c>
     </row>
-    <row r="34" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D34" s="6">
+    <row r="39" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D39" s="5">
         <v>1001</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H39" s="2">
         <v>39122</v>
       </c>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="6">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="6">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="6">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D38" s="6">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="6">
-        <v>1035</v>
-      </c>
-    </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>1036</v>
       </c>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>1037</v>
       </c>
     </row>
     <row r="42" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>1038</v>
       </c>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>1039</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>1040</v>
       </c>
     </row>
     <row r="45" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>1041</v>
       </c>
     </row>
     <row r="46" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>1042</v>
       </c>
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="6">
+      <c r="D47" s="5">
         <v>1043</v>
       </c>
     </row>
     <row r="48" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>1044</v>
       </c>
     </row>
@@ -1223,7 +1328,7 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <f>D$6+(D$7-D$6)*G14</f>
         <v>0.72</v>
       </c>
@@ -1236,7 +1341,7 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <f t="shared" ref="F15:F25" si="0">D$6+(D$7-D$6)*G15</f>
         <v>0.7823129545213815</v>
       </c>
@@ -1249,7 +1354,7 @@
       <c r="E16">
         <v>2</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <f t="shared" si="0"/>
         <v>0.82104127505777547</v>
       </c>
@@ -1262,7 +1367,7 @@
       <c r="E17">
         <v>3</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <f t="shared" si="0"/>
         <v>0.84921381875006041</v>
       </c>
@@ -1275,7 +1380,7 @@
       <c r="E18">
         <v>4</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <f t="shared" si="0"/>
         <v>0.87136924146659811</v>
       </c>
@@ -1288,7 +1393,7 @@
       <c r="E19">
         <v>5</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <f t="shared" si="0"/>
         <v>0.88963088204351404</v>
       </c>
@@ -1301,7 +1406,7 @@
       <c r="E20">
         <v>6</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <f t="shared" si="0"/>
         <v>0.90516496115631129</v>
       </c>
@@ -1314,7 +1419,7 @@
       <c r="E21">
         <v>7</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <f t="shared" si="0"/>
         <v>0.91868136829746028</v>
       </c>
@@ -1327,7 +1432,7 @@
       <c r="E22">
         <v>8</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <f t="shared" si="0"/>
         <v>0.93064449773228375</v>
       </c>
@@ -1340,7 +1445,7 @@
       <c r="E23">
         <v>9</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <f t="shared" si="0"/>
         <v>0.94137483412495926</v>
       </c>
@@ -1353,7 +1458,7 @@
       <c r="E24">
         <v>10</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <f t="shared" si="0"/>
         <v>0.9511028852698602</v>
       </c>
@@ -1366,7 +1471,7 @@
       <c r="E25">
         <v>11</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>

</xml_diff>

<commit_message>
Issue no. 68 @1413556783
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -274,6 +274,27 @@
   </si>
   <si>
     <t>16.09.2014: Notwendig für klassenspezifische Attribute, bspw. type, die nicht im Scope der Parent-Klasse BodyOrbitalType liegen.</t>
+  </si>
+  <si>
+    <t>PDF quer bei BodySun mit Dial an circle-Attribut</t>
+  </si>
+  <si>
+    <t>Ausgabe in gs korrekt.</t>
+  </si>
+  <si>
+    <t>BodyOrbitalType mit Dial an circle-Attribut und FOV-Intersection implementieren</t>
+  </si>
+  <si>
+    <t>division nur bei baseline="rail" erforderlich.</t>
+  </si>
+  <si>
+    <t>Konzept für Relation von baseline- un ddivision-Attributen von DialType.</t>
+  </si>
+  <si>
+    <t>Konzept für Relation von circle-Attribut und DIalType</t>
+  </si>
+  <si>
+    <t>circle als Attribut von DialType prüfen.</t>
   </si>
 </sst>
 </file>
@@ -649,10 +670,10 @@
   <dimension ref="D4:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,538 +703,571 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="4:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5" s="5">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H5" s="2">
-        <v>41924</v>
-      </c>
-      <c r="I5" s="2">
-        <v>41928</v>
-      </c>
-    </row>
-    <row r="6" spans="4:9" ht="60" x14ac:dyDescent="0.25">
+        <v>41929</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D6" s="5">
-        <v>1033</v>
+        <v>1037</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H6" s="2">
-        <v>41918</v>
+        <v>41929</v>
       </c>
     </row>
     <row r="7" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D7" s="5">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="H7" s="2">
-        <v>41918</v>
+        <v>41929</v>
       </c>
     </row>
     <row r="8" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D8" s="5">
-        <v>1031</v>
+        <v>1039</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="H8" s="2">
-        <v>41917</v>
-      </c>
-      <c r="I8" s="2">
+        <v>41929</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="D9" s="5">
+        <v>1035</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="2">
+        <v>41924</v>
+      </c>
+      <c r="I9" s="2">
         <v>41928</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D9" s="5">
-        <v>1032</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="2">
-        <v>41917</v>
       </c>
     </row>
     <row r="10" spans="4:9" ht="60" x14ac:dyDescent="0.25">
       <c r="D10" s="5">
-        <v>1030</v>
+        <v>1033</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="H10" s="2">
-        <v>41893</v>
-      </c>
-      <c r="I10" s="2">
-        <v>41924</v>
+        <v>41918</v>
       </c>
     </row>
     <row r="11" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D11" s="5">
-        <v>1028</v>
+        <v>1034</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2">
-        <v>41891</v>
-      </c>
-      <c r="I11" s="2">
-        <v>41895</v>
-      </c>
-    </row>
-    <row r="12" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+        <v>41918</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D12" s="5">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="H12" s="2">
-        <v>41891</v>
+        <v>41917</v>
       </c>
       <c r="I12" s="2">
         <v>41928</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
+        <v>1032</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="2">
+        <v>41917</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="D14" s="5">
+        <v>1030</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="2">
+        <v>41893</v>
+      </c>
+      <c r="I14" s="2">
+        <v>41924</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D15" s="5">
+        <v>1028</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="2">
+        <v>41891</v>
+      </c>
+      <c r="I15" s="2">
+        <v>41895</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="5">
+        <v>1029</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="2">
+        <v>41891</v>
+      </c>
+      <c r="I16" s="2">
+        <v>41928</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="5">
         <v>1025</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H17" s="2">
         <v>41869</v>
       </c>
     </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="5">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="5">
         <v>1022</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H18" s="2">
         <v>41854</v>
       </c>
     </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="5">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="5">
         <v>1023</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H19" s="2">
         <v>41854</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I19" s="2">
         <v>41891</v>
       </c>
     </row>
-    <row r="16" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D16" s="5">
+    <row r="20" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D20" s="5">
         <v>1024</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H20" s="2">
         <v>41854</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D17" s="5">
+    <row r="21" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="5">
         <v>1026</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H21" s="2">
         <v>41841</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I21" s="2">
         <v>41901</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D18" s="5">
+    <row r="22" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" s="5">
         <v>1027</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H22" s="2">
         <v>41841</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I22" s="2">
         <v>41901</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D19" s="5">
+    <row r="23" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D23" s="5">
         <v>1019</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H23" s="2">
         <v>41724</v>
       </c>
     </row>
-    <row r="20" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D20" s="5">
+    <row r="24" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D24" s="5">
         <v>1020</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H24" s="2">
         <v>41724</v>
       </c>
     </row>
-    <row r="21" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D21" s="5">
+    <row r="25" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D25" s="5">
         <v>1021</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H25" s="2">
         <v>41724</v>
       </c>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="5">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="5">
         <v>1018</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H26" s="2">
         <v>41576</v>
       </c>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="5">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="5">
         <v>1017</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H27" s="2">
         <v>41484</v>
-      </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="5">
-        <v>1016</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="2">
-        <v>41363</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D25" s="5">
-        <v>1015</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H25" s="2">
-        <v>41362</v>
-      </c>
-    </row>
-    <row r="26" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D26" s="5">
-        <v>1014</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="2">
-        <v>41229</v>
-      </c>
-    </row>
-    <row r="27" spans="4:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="D27" s="5">
-        <v>1013</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H27" s="2">
-        <v>41092</v>
       </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28" s="5">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H28" s="2">
-        <v>41028</v>
+        <v>41363</v>
       </c>
     </row>
     <row r="29" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D29" s="5">
+        <v>1015</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="2">
+        <v>41362</v>
+      </c>
+    </row>
+    <row r="30" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D30" s="5">
+        <v>1014</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="2">
+        <v>41229</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="D31" s="5">
+        <v>1013</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H31" s="2">
+        <v>41092</v>
+      </c>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="5">
+        <v>1012</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="2">
+        <v>41028</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D33" s="5">
         <v>1010</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H33" s="2">
         <v>40959</v>
       </c>
     </row>
-    <row r="30" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D30" s="5">
+    <row r="34" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D34" s="5">
         <v>1011</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H34" s="2">
         <v>40959</v>
       </c>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="5">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D35" s="5">
         <v>1008</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H35" s="2">
         <v>40956</v>
       </c>
     </row>
-    <row r="32" spans="4:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="D32" s="5">
+    <row r="36" spans="4:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="D36" s="5">
         <v>1009</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H36" s="2">
         <v>40956</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="5">
-        <v>1007</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" s="2">
-        <v>40947</v>
-      </c>
-    </row>
-    <row r="34" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D34" s="5">
-        <v>1006</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="2">
-        <v>40869</v>
-      </c>
-    </row>
-    <row r="35" spans="4:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="D35" s="5">
-        <v>1005</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H35" s="2">
-        <v>40866</v>
-      </c>
-    </row>
-    <row r="36" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D36" s="5">
-        <v>1004</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="2">
-        <v>40794</v>
       </c>
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" s="5">
-        <v>1003</v>
+        <v>1007</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H37" s="2">
-        <v>40763</v>
-      </c>
-    </row>
-    <row r="38" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+        <v>40947</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D38" s="5">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H38" s="2">
-        <v>40506</v>
-      </c>
-    </row>
-    <row r="39" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+        <v>40869</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" ht="90" x14ac:dyDescent="0.25">
       <c r="D39" s="5">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H39" s="2">
-        <v>39122</v>
-      </c>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
+        <v>40866</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D40" s="5">
-        <v>1036</v>
+        <v>1004</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="2">
+        <v>40794</v>
       </c>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41" s="5">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
+        <v>1003</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" s="2">
+        <v>40763</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D42" s="5">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
+        <v>1002</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="2">
+        <v>40506</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D43" s="5">
-        <v>1039</v>
+        <v>1001</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="2">
+        <v>39122</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Issue no. 71 @1419183165
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>03.08.2014: Nord-/ Südhimmel prüfen.</t>
-  </si>
-  <si>
-    <t>Optional, Default-Wert true.</t>
   </si>
   <si>
     <t>Optional, Default-Wert false.</t>
@@ -210,9 +207,6 @@
     <t>Klasse ist Alpha, Omega optional, Mapping wegen Namenskonflikt mit Circle* einführen.</t>
   </si>
   <si>
-    <t>Alpha/ Omega optional, default 0/ 359 bzw. -90/ 90 (prefs), mapping wegen Namenskonflikt mit Epoch einführen</t>
-  </si>
-  <si>
     <t>Klasse Epoch optimieren</t>
   </si>
   <si>
@@ -220,9 +214,6 @@
   </si>
   <si>
     <t>CircleType Begin/ End nach Alpha/ Omega ändern</t>
-  </si>
-  <si>
-    <t>Element-Class-mapping, beide optional, default aus preferences.</t>
   </si>
   <si>
     <t>Differenzierung von preferences für GraduationSpan, -Half, -Full über name-Attribut, division-Attribut von GraduationSpan nach DialDegree ändern.</t>
@@ -294,6 +285,12 @@
   </si>
   <si>
     <t>Attribut circle von BodyOrbitalType als baseline nach DialType migrieren</t>
+  </si>
+  <si>
+    <t>Element-Class-mapping, beide optional, default (0/ 359,99 bzw. -85/ 85) aus preferences, mapping wegen Namenskonflikt mit Epoch einführen.</t>
+  </si>
+  <si>
+    <t>Optional, Default-Wert true. Alternativ contour-Attribut von CatalogDS9Record prüfen.</t>
   </si>
 </sst>
 </file>
@@ -666,7 +663,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +698,7 @@
         <v>1042</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H5" s="2">
         <v>41948</v>
@@ -712,7 +709,7 @@
         <v>1043</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H6" s="2">
         <v>41948</v>
@@ -723,10 +720,10 @@
         <v>1040</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H7" s="2">
         <v>41941</v>
@@ -737,13 +734,13 @@
         <v>1041</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H8" s="2">
         <v>41941</v>
@@ -754,10 +751,10 @@
         <v>1036</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H9" s="2">
         <v>41929</v>
@@ -768,10 +765,10 @@
         <v>1037</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H10" s="2">
         <v>41929</v>
@@ -785,13 +782,13 @@
         <v>1035</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H11" s="2">
         <v>41924</v>
@@ -805,10 +802,10 @@
         <v>1038</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H12" s="2">
         <v>41929</v>
@@ -822,10 +819,10 @@
         <v>1039</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H13" s="2">
         <v>41929</v>
@@ -839,10 +836,10 @@
         <v>1031</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="2">
         <v>41917</v>
@@ -856,10 +853,10 @@
         <v>1033</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H15" s="2">
         <v>41918</v>
@@ -870,10 +867,10 @@
         <v>1030</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H16" s="2">
         <v>41893</v>
@@ -887,13 +884,13 @@
         <v>1028</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H17" s="2">
         <v>41891</v>
@@ -907,10 +904,10 @@
         <v>1029</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H18" s="2">
         <v>41891</v>
@@ -919,29 +916,26 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D19" s="5">
         <v>1034</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="H19" s="2">
         <v>41918</v>
       </c>
     </row>
-    <row r="20" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20" s="5">
         <v>1032</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H20" s="2">
         <v>41917</v>
@@ -952,10 +946,10 @@
         <v>1023</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="2">
         <v>41854</v>
@@ -969,10 +963,10 @@
         <v>1025</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="2">
         <v>41869</v>
@@ -983,10 +977,10 @@
         <v>1026</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H23" s="2">
         <v>41841</v>
@@ -1000,13 +994,13 @@
         <v>1027</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H24" s="2">
         <v>41841</v>
@@ -1015,15 +1009,15 @@
         <v>41901</v>
       </c>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D25" s="5">
         <v>1022</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="H25" s="2">
         <v>41854</v>
@@ -1034,10 +1028,10 @@
         <v>1024</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="H26" s="2">
         <v>41854</v>
@@ -1199,7 +1193,7 @@
         <v>13</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H38" s="2">
         <v>40959</v>
@@ -1266,7 +1260,7 @@
         <v>24</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" s="2">
         <v>40866</v>

</xml_diff>

<commit_message>
Issue no. 74 @1432056729
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -361,9 +361,6 @@
     <t>astrolabe.Coordinate.spherical/ .cartesian einführen.</t>
   </si>
   <si>
-    <t>11.03.2015: P4 Klassen in C++ für CUDA, Java per JNI.</t>
-  </si>
-  <si>
     <t>15.03.2015: Tabelle test files, Tabelle test sets.</t>
   </si>
   <si>
@@ -387,6 +384,10 @@
   <si>
     <t>26.03.2015: Google: segmentation of astronomical images.
 27.03.2015: Google: sextractor.</t>
+  </si>
+  <si>
+    <t>11.03.2015: P4 Klassen in C++ für CUDA, Java per JNI.
+19.05.2015: Java 7 x86_64 installiert.</t>
   </si>
 </sst>
 </file>
@@ -756,10 +757,10 @@
   <dimension ref="D4:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,10 +832,10 @@
         <v>1054</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H7" s="2">
         <v>42084</v>
@@ -885,7 +886,7 @@
         <v>1052</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H10" s="2">
         <v>42081</v>
@@ -899,13 +900,13 @@
         <v>1053</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H11" s="2">
         <v>42081</v>
@@ -1196,7 +1197,7 @@
         <v>73</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H29" s="2">
         <v>41941</v>
@@ -1337,7 +1338,7 @@
         <v>33</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="H38" s="2">
         <v>41724</v>
@@ -1575,7 +1576,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H55" s="2">
         <v>40794</v>

</xml_diff>